<commit_message>
add reed CH data exploration
</commit_message>
<xml_diff>
--- a/database_exploration/clickhouse/benchmark/output/load_benchmark_results.xlsx
+++ b/database_exploration/clickhouse/benchmark/output/load_benchmark_results.xlsx
@@ -7,7 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="WRITE" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="REED" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -177,7 +178,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D1</f>
+              <f>'WRITE'!D1</f>
             </strRef>
           </tx>
           <spPr>
@@ -187,12 +188,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Sheet'!$A$2:$A$7</f>
+              <f>'WRITE'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$D$2:$D$7</f>
+              <f>'WRITE'!$D$2:$D$7</f>
             </numRef>
           </val>
         </ser>
@@ -289,7 +290,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D1</f>
+              <f>'WRITE'!D1</f>
             </strRef>
           </tx>
           <spPr>
@@ -299,12 +300,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Sheet'!$A$2:$A$7</f>
+              <f>'WRITE'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$D$2:$D$7</f>
+              <f>'WRITE'!$D$2:$D$7</f>
             </numRef>
           </val>
         </ser>
@@ -401,7 +402,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D7</f>
+              <f>'WRITE'!D7</f>
             </strRef>
           </tx>
           <spPr>
@@ -411,12 +412,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Sheet'!$A$8:$A$13</f>
+              <f>'WRITE'!$A$8:$A$13</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$D$8:$D$13</f>
+              <f>'WRITE'!$D$8:$D$13</f>
             </numRef>
           </val>
         </ser>
@@ -512,7 +513,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D1</f>
+              <f>'WRITE'!D1</f>
             </strRef>
           </tx>
           <spPr>
@@ -530,7 +531,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Sheet'!$D$2:$D$7</f>
+              <f>'WRITE'!$D$2:$D$7</f>
             </numRef>
           </val>
         </ser>
@@ -539,7 +540,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D7</f>
+              <f>'WRITE'!D7</f>
             </strRef>
           </tx>
           <spPr>
@@ -557,7 +558,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Sheet'!$D$8:$D$13</f>
+              <f>'WRITE'!$D$8:$D$13</f>
             </numRef>
           </val>
         </ser>
@@ -653,7 +654,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D1</f>
+              <f>'WRITE'!D1</f>
             </strRef>
           </tx>
           <spPr>
@@ -663,12 +664,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Sheet'!$A$2:$A$7</f>
+              <f>'WRITE'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$D$2:$D$7</f>
+              <f>'WRITE'!$D$2:$D$7</f>
             </numRef>
           </val>
         </ser>
@@ -765,7 +766,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D7</f>
+              <f>'WRITE'!D7</f>
             </strRef>
           </tx>
           <spPr>
@@ -775,12 +776,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Sheet'!$A$8:$A$13</f>
+              <f>'WRITE'!$A$8:$A$13</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$D$8:$D$13</f>
+              <f>'WRITE'!$D$8:$D$13</f>
             </numRef>
           </val>
         </ser>
@@ -876,7 +877,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D1</f>
+              <f>'WRITE'!D1</f>
             </strRef>
           </tx>
           <spPr>
@@ -894,7 +895,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Sheet'!$D$2:$D$7</f>
+              <f>'WRITE'!$D$2:$D$7</f>
             </numRef>
           </val>
         </ser>
@@ -903,7 +904,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D7</f>
+              <f>'WRITE'!D7</f>
             </strRef>
           </tx>
           <spPr>
@@ -921,7 +922,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Sheet'!$D$8:$D$13</f>
+              <f>'WRITE'!$D$8:$D$13</f>
             </numRef>
           </val>
         </ser>
@@ -1017,7 +1018,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D1</f>
+              <f>'WRITE'!D1</f>
             </strRef>
           </tx>
           <spPr>
@@ -1027,12 +1028,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Sheet'!$A$2:$A$7</f>
+              <f>'WRITE'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$D$2:$D$7</f>
+              <f>'WRITE'!$D$2:$D$7</f>
             </numRef>
           </val>
         </ser>
@@ -1129,7 +1130,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D7</f>
+              <f>'WRITE'!D7</f>
             </strRef>
           </tx>
           <spPr>
@@ -1139,12 +1140,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Sheet'!$A$8:$A$13</f>
+              <f>'WRITE'!$A$8:$A$13</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$D$8:$D$13</f>
+              <f>'WRITE'!$D$8:$D$13</f>
             </numRef>
           </val>
         </ser>
@@ -1240,7 +1241,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D1</f>
+              <f>'WRITE'!D1</f>
             </strRef>
           </tx>
           <spPr>
@@ -1258,7 +1259,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Sheet'!$D$2:$D$7</f>
+              <f>'WRITE'!$D$2:$D$7</f>
             </numRef>
           </val>
         </ser>
@@ -1267,7 +1268,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D7</f>
+              <f>'WRITE'!D7</f>
             </strRef>
           </tx>
           <spPr>
@@ -1285,7 +1286,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Sheet'!$D$8:$D$13</f>
+              <f>'WRITE'!$D$8:$D$13</f>
             </numRef>
           </val>
         </ser>
@@ -1381,7 +1382,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D1</f>
+              <f>'WRITE'!D1</f>
             </strRef>
           </tx>
           <spPr>
@@ -1391,12 +1392,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Sheet'!$A$2:$A$7</f>
+              <f>'WRITE'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$D$2:$D$7</f>
+              <f>'WRITE'!$D$2:$D$7</f>
             </numRef>
           </val>
         </ser>
@@ -1493,7 +1494,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D7</f>
+              <f>'WRITE'!D7</f>
             </strRef>
           </tx>
           <spPr>
@@ -1503,12 +1504,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Sheet'!$A$8:$A$13</f>
+              <f>'WRITE'!$A$8:$A$13</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$D$8:$D$13</f>
+              <f>'WRITE'!$D$8:$D$13</f>
             </numRef>
           </val>
         </ser>
@@ -1605,7 +1606,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D7</f>
+              <f>'WRITE'!D7</f>
             </strRef>
           </tx>
           <spPr>
@@ -1615,12 +1616,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Sheet'!$A$8:$A$13</f>
+              <f>'WRITE'!$A$8:$A$13</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$D$8:$D$13</f>
+              <f>'WRITE'!$D$8:$D$13</f>
             </numRef>
           </val>
         </ser>
@@ -1716,7 +1717,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D1</f>
+              <f>'WRITE'!D1</f>
             </strRef>
           </tx>
           <spPr>
@@ -1734,7 +1735,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Sheet'!$D$2:$D$7</f>
+              <f>'WRITE'!$D$2:$D$7</f>
             </numRef>
           </val>
         </ser>
@@ -1743,7 +1744,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D7</f>
+              <f>'WRITE'!D7</f>
             </strRef>
           </tx>
           <spPr>
@@ -1761,7 +1762,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Sheet'!$D$8:$D$13</f>
+              <f>'WRITE'!$D$8:$D$13</f>
             </numRef>
           </val>
         </ser>
@@ -1857,7 +1858,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D1</f>
+              <f>'WRITE'!D1</f>
             </strRef>
           </tx>
           <spPr>
@@ -1867,12 +1868,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Sheet'!$A$2:$A$7</f>
+              <f>'WRITE'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$D$2:$D$7</f>
+              <f>'WRITE'!$D$2:$D$7</f>
             </numRef>
           </val>
         </ser>
@@ -1969,7 +1970,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D7</f>
+              <f>'WRITE'!D7</f>
             </strRef>
           </tx>
           <spPr>
@@ -1979,12 +1980,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Sheet'!$A$8:$A$13</f>
+              <f>'WRITE'!$A$8:$A$13</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$D$8:$D$13</f>
+              <f>'WRITE'!$D$8:$D$13</f>
             </numRef>
           </val>
         </ser>
@@ -2080,7 +2081,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D1</f>
+              <f>'WRITE'!D1</f>
             </strRef>
           </tx>
           <spPr>
@@ -2098,7 +2099,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Sheet'!$D$2:$D$7</f>
+              <f>'WRITE'!$D$2:$D$7</f>
             </numRef>
           </val>
         </ser>
@@ -2107,7 +2108,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D7</f>
+              <f>'WRITE'!D7</f>
             </strRef>
           </tx>
           <spPr>
@@ -2125,7 +2126,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Sheet'!$D$8:$D$13</f>
+              <f>'WRITE'!$D$8:$D$13</f>
             </numRef>
           </val>
         </ser>
@@ -2221,7 +2222,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D1</f>
+              <f>'WRITE'!D1</f>
             </strRef>
           </tx>
           <spPr>
@@ -2231,12 +2232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Sheet'!$A$2:$A$7</f>
+              <f>'WRITE'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$D$2:$D$7</f>
+              <f>'WRITE'!$D$2:$D$7</f>
             </numRef>
           </val>
         </ser>
@@ -2333,7 +2334,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D7</f>
+              <f>'WRITE'!D7</f>
             </strRef>
           </tx>
           <spPr>
@@ -2343,12 +2344,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Sheet'!$A$8:$A$13</f>
+              <f>'WRITE'!$A$8:$A$13</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$D$8:$D$13</f>
+              <f>'WRITE'!$D$8:$D$13</f>
             </numRef>
           </val>
         </ser>
@@ -2444,7 +2445,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D1</f>
+              <f>'WRITE'!D1</f>
             </strRef>
           </tx>
           <spPr>
@@ -2462,7 +2463,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Sheet'!$D$2:$D$7</f>
+              <f>'WRITE'!$D$2:$D$7</f>
             </numRef>
           </val>
         </ser>
@@ -2471,7 +2472,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D7</f>
+              <f>'WRITE'!D7</f>
             </strRef>
           </tx>
           <spPr>
@@ -2489,7 +2490,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Sheet'!$D$8:$D$13</f>
+              <f>'WRITE'!$D$8:$D$13</f>
             </numRef>
           </val>
         </ser>
@@ -2585,7 +2586,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D1</f>
+              <f>'WRITE'!D1</f>
             </strRef>
           </tx>
           <spPr>
@@ -2595,12 +2596,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Sheet'!$A$2:$A$7</f>
+              <f>'WRITE'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$D$2:$D$7</f>
+              <f>'WRITE'!$D$2:$D$7</f>
             </numRef>
           </val>
         </ser>
@@ -2697,7 +2698,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D7</f>
+              <f>'WRITE'!D7</f>
             </strRef>
           </tx>
           <spPr>
@@ -2707,12 +2708,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Sheet'!$A$8:$A$13</f>
+              <f>'WRITE'!$A$8:$A$13</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$D$8:$D$13</f>
+              <f>'WRITE'!$D$8:$D$13</f>
             </numRef>
           </val>
         </ser>
@@ -2808,7 +2809,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D1</f>
+              <f>'WRITE'!D1</f>
             </strRef>
           </tx>
           <spPr>
@@ -2826,7 +2827,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Sheet'!$D$2:$D$7</f>
+              <f>'WRITE'!$D$2:$D$7</f>
             </numRef>
           </val>
         </ser>
@@ -2835,7 +2836,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D7</f>
+              <f>'WRITE'!D7</f>
             </strRef>
           </tx>
           <spPr>
@@ -2853,7 +2854,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Sheet'!$D$8:$D$13</f>
+              <f>'WRITE'!$D$8:$D$13</f>
             </numRef>
           </val>
         </ser>
@@ -2948,7 +2949,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D1</f>
+              <f>'WRITE'!D1</f>
             </strRef>
           </tx>
           <spPr>
@@ -2966,7 +2967,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Sheet'!$D$2:$D$7</f>
+              <f>'WRITE'!$D$2:$D$7</f>
             </numRef>
           </val>
         </ser>
@@ -2975,7 +2976,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D7</f>
+              <f>'WRITE'!D7</f>
             </strRef>
           </tx>
           <spPr>
@@ -2993,7 +2994,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Sheet'!$D$8:$D$13</f>
+              <f>'WRITE'!$D$8:$D$13</f>
             </numRef>
           </val>
         </ser>
@@ -3089,7 +3090,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D1</f>
+              <f>'WRITE'!D1</f>
             </strRef>
           </tx>
           <spPr>
@@ -3099,12 +3100,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Sheet'!$A$2:$A$7</f>
+              <f>'WRITE'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$D$2:$D$7</f>
+              <f>'WRITE'!$D$2:$D$7</f>
             </numRef>
           </val>
         </ser>
@@ -3201,7 +3202,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D7</f>
+              <f>'WRITE'!D7</f>
             </strRef>
           </tx>
           <spPr>
@@ -3211,12 +3212,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Sheet'!$A$8:$A$13</f>
+              <f>'WRITE'!$A$8:$A$13</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$D$8:$D$13</f>
+              <f>'WRITE'!$D$8:$D$13</f>
             </numRef>
           </val>
         </ser>
@@ -3312,7 +3313,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D1</f>
+              <f>'WRITE'!D1</f>
             </strRef>
           </tx>
           <spPr>
@@ -3330,7 +3331,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Sheet'!$D$2:$D$7</f>
+              <f>'WRITE'!$D$2:$D$7</f>
             </numRef>
           </val>
         </ser>
@@ -3339,7 +3340,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D7</f>
+              <f>'WRITE'!D7</f>
             </strRef>
           </tx>
           <spPr>
@@ -3357,7 +3358,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Sheet'!$D$8:$D$13</f>
+              <f>'WRITE'!$D$8:$D$13</f>
             </numRef>
           </val>
         </ser>
@@ -3453,7 +3454,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D1</f>
+              <f>'WRITE'!D1</f>
             </strRef>
           </tx>
           <spPr>
@@ -3463,12 +3464,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Sheet'!$A$2:$A$7</f>
+              <f>'WRITE'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$D$2:$D$7</f>
+              <f>'WRITE'!$D$2:$D$7</f>
             </numRef>
           </val>
         </ser>
@@ -3565,7 +3566,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D7</f>
+              <f>'WRITE'!D7</f>
             </strRef>
           </tx>
           <spPr>
@@ -3575,12 +3576,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Sheet'!$A$8:$A$13</f>
+              <f>'WRITE'!$A$8:$A$13</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$D$8:$D$13</f>
+              <f>'WRITE'!$D$8:$D$13</f>
             </numRef>
           </val>
         </ser>
@@ -3676,7 +3677,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D1</f>
+              <f>'WRITE'!D1</f>
             </strRef>
           </tx>
           <spPr>
@@ -3694,7 +3695,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Sheet'!$D$2:$D$7</f>
+              <f>'WRITE'!$D$2:$D$7</f>
             </numRef>
           </val>
         </ser>
@@ -3703,7 +3704,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D7</f>
+              <f>'WRITE'!D7</f>
             </strRef>
           </tx>
           <spPr>
@@ -3721,13 +3722,349 @@
           </marker>
           <val>
             <numRef>
-              <f>'Sheet'!$D$8:$D$13</f>
+              <f>'WRITE'!$D$8:$D$13</f>
             </numRef>
           </val>
         </ser>
         <axId val="10"/>
         <axId val="100"/>
       </lineChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>кол-во записей</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>скорость записи/сек</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart37.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Скорость чтения</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'REED'!B1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'REED'!$A$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'REED'!$B$2</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>кол-во записей</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>скорость записи/сек</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart38.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Скорость чтения</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'REED'!B1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'REED'!$A$2:$A$3</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'REED'!$B$2:$B$3</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>кол-во записей</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>скорость записи/сек</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart39.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Скорость чтения</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'REED'!B1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'REED'!$A$2:$A$4</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'REED'!$B$2:$B$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
       <catAx>
         <axId val="10"/>
         <scaling>
@@ -3817,7 +4154,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D1</f>
+              <f>'WRITE'!D1</f>
             </strRef>
           </tx>
           <spPr>
@@ -3827,12 +4164,908 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Sheet'!$A$2:$A$7</f>
+              <f>'WRITE'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$D$2:$D$7</f>
+              <f>'WRITE'!$D$2:$D$7</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>кол-во записей</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>скорость записи/сек</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart40.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Скорость чтения</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'REED'!B1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'REED'!$A$2:$A$5</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'REED'!$B$2:$B$5</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>кол-во записей</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>скорость записи/сек</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart41.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Скорость чтения</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'REED'!B1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'REED'!$A$2:$A$6</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'REED'!$B$2:$B$6</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>кол-во записей</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>скорость записи/сек</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart42.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Скорость чтения</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'REED'!B1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'REED'!$A$2:$A$7</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'REED'!$B$2:$B$7</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>кол-во записей</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>скорость записи/сек</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart43.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Скорость чтения</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'REED'!B1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'REED'!$A$2:$A$8</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'REED'!$B$2:$B$8</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>кол-во записей</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>скорость записи/сек</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart44.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Скорость чтения</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'REED'!B1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'REED'!$A$2:$A$9</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'REED'!$B$2:$B$9</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>кол-во записей</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>скорость записи/сек</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart45.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Скорость чтения</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'REED'!B1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'REED'!$A$2:$A$10</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'REED'!$B$2:$B$10</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>кол-во записей</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>скорость записи/сек</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart46.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Скорость чтения</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'REED'!B1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'REED'!$A$2:$A$11</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'REED'!$B$2:$B$11</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>кол-во записей</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>скорость записи/сек</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart47.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Скорость чтения</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="standard"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'REED'!B1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'REED'!$A$2:$A$12</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'REED'!$B$2:$B$12</f>
             </numRef>
           </val>
         </ser>
@@ -3929,7 +5162,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D7</f>
+              <f>'WRITE'!D7</f>
             </strRef>
           </tx>
           <spPr>
@@ -3939,12 +5172,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Sheet'!$A$8:$A$13</f>
+              <f>'WRITE'!$A$8:$A$13</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$D$8:$D$13</f>
+              <f>'WRITE'!$D$8:$D$13</f>
             </numRef>
           </val>
         </ser>
@@ -4040,7 +5273,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D1</f>
+              <f>'WRITE'!D1</f>
             </strRef>
           </tx>
           <spPr>
@@ -4058,7 +5291,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Sheet'!$D$2:$D$7</f>
+              <f>'WRITE'!$D$2:$D$7</f>
             </numRef>
           </val>
         </ser>
@@ -4067,7 +5300,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D7</f>
+              <f>'WRITE'!D7</f>
             </strRef>
           </tx>
           <spPr>
@@ -4085,7 +5318,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Sheet'!$D$8:$D$13</f>
+              <f>'WRITE'!$D$8:$D$13</f>
             </numRef>
           </val>
         </ser>
@@ -4181,7 +5414,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D1</f>
+              <f>'WRITE'!D1</f>
             </strRef>
           </tx>
           <spPr>
@@ -4191,12 +5424,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Sheet'!$A$2:$A$7</f>
+              <f>'WRITE'!$A$2:$A$7</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$D$2:$D$7</f>
+              <f>'WRITE'!$D$2:$D$7</f>
             </numRef>
           </val>
         </ser>
@@ -4293,7 +5526,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D7</f>
+              <f>'WRITE'!D7</f>
             </strRef>
           </tx>
           <spPr>
@@ -4303,12 +5536,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Sheet'!$A$8:$A$13</f>
+              <f>'WRITE'!$A$8:$A$13</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sheet'!$D$8:$D$13</f>
+              <f>'WRITE'!$D$8:$D$13</f>
             </numRef>
           </val>
         </ser>
@@ -4404,7 +5637,7 @@
           <order val="0"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D1</f>
+              <f>'WRITE'!D1</f>
             </strRef>
           </tx>
           <spPr>
@@ -4422,7 +5655,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Sheet'!$D$2:$D$7</f>
+              <f>'WRITE'!$D$2:$D$7</f>
             </numRef>
           </val>
         </ser>
@@ -4431,7 +5664,7 @@
           <order val="1"/>
           <tx>
             <strRef>
-              <f>'Sheet'!D7</f>
+              <f>'WRITE'!D7</f>
             </strRef>
           </tx>
           <spPr>
@@ -4449,7 +5682,7 @@
           </marker>
           <val>
             <numRef>
-              <f>'Sheet'!$D$8:$D$13</f>
+              <f>'WRITE'!$D$8:$D$13</f>
             </numRef>
           </val>
         </ser>
@@ -5315,6 +6548,253 @@
 </wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="2" name="Chart 2"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="3" name="Chart 3"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="4" name="Chart 4"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="5" name="Chart 5"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="6" name="Chart 6"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="7" name="Chart 7"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="8" name="Chart 8"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="9" name="Chart 9"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="10" name="Chart 10"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId10"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="11" name="Chart 11"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId11"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5672,16 +7152,16 @@
         <v>10000</v>
       </c>
       <c r="C2" t="n">
-        <v>0.02839422225952148</v>
+        <v>0.03597068786621094</v>
       </c>
       <c r="D2" t="n">
-        <v>176092</v>
+        <v>139002</v>
       </c>
       <c r="E2" t="n">
-        <v>2484</v>
+        <v>2522</v>
       </c>
       <c r="F2" t="n">
-        <v>2516</v>
+        <v>2478</v>
       </c>
     </row>
     <row r="3">
@@ -5692,16 +7172,16 @@
         <v>10000</v>
       </c>
       <c r="C3" t="n">
-        <v>0.04664087295532227</v>
+        <v>0.08447098731994629</v>
       </c>
       <c r="D3" t="n">
-        <v>214404</v>
+        <v>118384</v>
       </c>
       <c r="E3" t="n">
-        <v>5008</v>
+        <v>5065</v>
       </c>
       <c r="F3" t="n">
-        <v>4992</v>
+        <v>4935</v>
       </c>
     </row>
     <row r="4">
@@ -5712,16 +7192,16 @@
         <v>10000</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4623169898986816</v>
+        <v>0.7307248115539551</v>
       </c>
       <c r="D4" t="n">
-        <v>216302</v>
+        <v>136850</v>
       </c>
       <c r="E4" t="n">
-        <v>50095</v>
+        <v>50296</v>
       </c>
       <c r="F4" t="n">
-        <v>49905</v>
+        <v>49704</v>
       </c>
     </row>
     <row r="5">
@@ -5732,16 +7212,16 @@
         <v>10000</v>
       </c>
       <c r="C5" t="n">
-        <v>2.476893186569214</v>
+        <v>3.827020406723022</v>
       </c>
       <c r="D5" t="n">
-        <v>201866</v>
+        <v>130650</v>
       </c>
       <c r="E5" t="n">
-        <v>249836</v>
+        <v>249172</v>
       </c>
       <c r="F5" t="n">
-        <v>250164</v>
+        <v>250828</v>
       </c>
     </row>
     <row r="6">
@@ -5752,16 +7232,16 @@
         <v>10000</v>
       </c>
       <c r="C6" t="n">
-        <v>6.946522235870361</v>
+        <v>7.436813116073608</v>
       </c>
       <c r="D6" t="n">
-        <v>143957</v>
+        <v>134466</v>
       </c>
       <c r="E6" t="n">
-        <v>499989</v>
+        <v>499929</v>
       </c>
       <c r="F6" t="n">
-        <v>500011</v>
+        <v>500071</v>
       </c>
     </row>
     <row r="7">
@@ -5772,16 +7252,16 @@
         <v>10000</v>
       </c>
       <c r="C7" t="n">
-        <v>23.27093625068665</v>
+        <v>30.40963673591614</v>
       </c>
       <c r="D7" t="n">
-        <v>171888</v>
+        <v>131537</v>
       </c>
       <c r="E7" t="n">
-        <v>1998423</v>
+        <v>2000956</v>
       </c>
       <c r="F7" t="n">
-        <v>2001577</v>
+        <v>1999044</v>
       </c>
     </row>
     <row r="8">
@@ -5792,16 +7272,16 @@
         <v>100000</v>
       </c>
       <c r="C8" t="n">
-        <v>0.03142237663269043</v>
+        <v>0.03312015533447266</v>
       </c>
       <c r="D8" t="n">
-        <v>159122</v>
+        <v>150965</v>
       </c>
       <c r="E8" t="n">
-        <v>2491</v>
+        <v>2501</v>
       </c>
       <c r="F8" t="n">
-        <v>2509</v>
+        <v>2499</v>
       </c>
     </row>
     <row r="9">
@@ -5812,16 +7292,16 @@
         <v>100000</v>
       </c>
       <c r="C9" t="n">
-        <v>0.04271769523620605</v>
+        <v>0.06108665466308594</v>
       </c>
       <c r="D9" t="n">
-        <v>234095</v>
+        <v>163702</v>
       </c>
       <c r="E9" t="n">
-        <v>5035</v>
+        <v>5144</v>
       </c>
       <c r="F9" t="n">
-        <v>4965</v>
+        <v>4856</v>
       </c>
     </row>
     <row r="10">
@@ -5832,16 +7312,16 @@
         <v>100000</v>
       </c>
       <c r="C10" t="n">
-        <v>0.4783587455749512</v>
+        <v>0.6597869396209717</v>
       </c>
       <c r="D10" t="n">
-        <v>209048</v>
+        <v>151564</v>
       </c>
       <c r="E10" t="n">
-        <v>49916</v>
+        <v>50064</v>
       </c>
       <c r="F10" t="n">
-        <v>50084</v>
+        <v>49936</v>
       </c>
     </row>
     <row r="11">
@@ -5852,16 +7332,16 @@
         <v>100000</v>
       </c>
       <c r="C11" t="n">
-        <v>2.330848932266235</v>
+        <v>3.313808441162109</v>
       </c>
       <c r="D11" t="n">
-        <v>214514</v>
+        <v>150884</v>
       </c>
       <c r="E11" t="n">
-        <v>249956</v>
+        <v>249540</v>
       </c>
       <c r="F11" t="n">
-        <v>250044</v>
+        <v>250460</v>
       </c>
     </row>
     <row r="12">
@@ -5872,16 +7352,16 @@
         <v>100000</v>
       </c>
       <c r="C12" t="n">
-        <v>4.790394067764282</v>
+        <v>6.888978481292725</v>
       </c>
       <c r="D12" t="n">
-        <v>208751</v>
+        <v>145159</v>
       </c>
       <c r="E12" t="n">
-        <v>499771</v>
+        <v>500303</v>
       </c>
       <c r="F12" t="n">
-        <v>500229</v>
+        <v>499697</v>
       </c>
     </row>
     <row r="13">
@@ -5892,16 +7372,218 @@
         <v>100000</v>
       </c>
       <c r="C13" t="n">
-        <v>18.23332953453064</v>
+        <v>28.23058152198792</v>
       </c>
       <c r="D13" t="n">
-        <v>219378</v>
+        <v>141690</v>
       </c>
       <c r="E13" t="n">
-        <v>2000921</v>
+        <v>1999112</v>
       </c>
       <c r="F13" t="n">
-        <v>1999079</v>
+        <v>2000888</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="13" customWidth="1" min="1" max="1"/>
+    <col width="13" customWidth="1" min="2" max="2"/>
+    <col width="13" customWidth="1" min="3" max="3"/>
+    <col width="13" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>rows_count</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>speed</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>stress</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>all data DB cnt</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>500000</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1476361</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1459353</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>100000</v>
+      </c>
+      <c r="B4" t="n">
+        <v>774077</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>4000000</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>500000</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1414188</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>4000000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1365772</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4000000</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>2000000</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1413523</v>
+      </c>
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>4000000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>4000000</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1589161</v>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>4000000</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>3000000</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1428964</v>
+      </c>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>4000000</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2000000</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1446750</v>
+      </c>
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" t="n">
+        <v>4000000</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>4000000</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1631738</v>
+      </c>
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" t="n">
+        <v>4000000</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>4000000</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1654013</v>
+      </c>
+      <c r="C12" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" t="n">
+        <v>4000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>